<commit_message>
Add references for gp.
</commit_message>
<xml_diff>
--- a/data/gp_asmt_create.xlsx
+++ b/data/gp_asmt_create.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19321"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ACC3FD1-6C72-452A-8AEF-95EB733087AA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancy/Study/bigben/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26000" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -29,42 +38,67 @@
     <t>grade_type</t>
   </si>
   <si>
-    <t>instruction</t>
-  </si>
-  <si>
-    <t>group_formads</t>
-  </si>
-  <si>
     <t>0001_Ren_GP</t>
   </si>
   <si>
-    <t>Five</t>
-  </si>
-  <si>
-    <t>Abc def</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
     <t>0002_Ren_GP</t>
   </si>
   <si>
     <t>A 2</t>
   </si>
   <si>
-    <t>BBB</t>
+    <t>Five Star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A 1</t>
+  </si>
+  <si>
+    <t>This message is post submission instructions text.</t>
+  </si>
+  <si>
+    <t>This message is instructions text.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instructions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_sub_instructions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Educator Formed</t>
+  </si>
+  <si>
+    <t>System Formed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_formed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -405,24 +439,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.25" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,18 +470,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>43213</v>
@@ -456,33 +493,40 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>43219</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bring in DeleteAsmtTest case.
</commit_message>
<xml_diff>
--- a/data/gp_asmt_create.xlsx
+++ b/data/gp_asmt_create.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancy/Study/bigben/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="26000" windowHeight="11160"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="25995" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -38,15 +33,6 @@
     <t>grade_type</t>
   </si>
   <si>
-    <t>0001_Ren_GP</t>
-  </si>
-  <si>
-    <t>0002_Ren_GP</t>
-  </si>
-  <si>
-    <t>A 2</t>
-  </si>
-  <si>
     <t>Five Star</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,9 +41,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A 1</t>
-  </si>
-  <si>
     <t>This message is post submission instructions text.</t>
   </si>
   <si>
@@ -82,6 +65,12 @@
   <si>
     <t>group_formed</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ren_GP_0001</t>
+  </si>
+  <si>
+    <t>Ren_GP_0002</t>
   </si>
 </sst>
 </file>
@@ -92,13 +81,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,7 +117,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -186,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -238,7 +227,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -432,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,20 +432,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,63 +459,64 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>43213</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>43219</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Suite for 3 asmts
</commit_message>
<xml_diff>
--- a/data/gp_asmt_create.xlsx
+++ b/data/gp_asmt_create.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancy/Study/bigben/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="25995" windowHeight="11160"/>
+    <workbookView xWindow="12040" yWindow="2920" windowWidth="26000" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -37,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>This message is post submission instructions text.</t>
   </si>
   <si>
@@ -59,18 +60,12 @@
     <t>Educator Formed</t>
   </si>
   <si>
-    <t>System Formed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>group_formed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Ren_GP_0001</t>
-  </si>
-  <si>
-    <t>Ren_GP_0002</t>
+    <t>Ren_GP_0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -81,13 +76,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -117,7 +112,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -421,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,20 +427,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,21 +454,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>43213</v>
@@ -482,37 +477,17 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43219</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>